<commit_message>
down up file ok
</commit_message>
<xml_diff>
--- a/templates/sample-danhmuc-tochuc.xlsx
+++ b/templates/sample-danhmuc-tochuc.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DINHNV\MyData\LAPTRINH\NODE4\ionic4.qlns\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331BE2E2-6F81-49E5-8E9C-AD3FA73E9223}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967B50F2-9D6E-4F56-8BDB-039CB5EEF459}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10695" yWindow="345" windowWidth="14535" windowHeight="12405" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="495" windowWidth="14535" windowHeight="12405" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="organizations" sheetId="16" r:id="rId1"/>
     <sheet name="job_roles" sheetId="18" r:id="rId2"/>
     <sheet name="staffs" sheetId="19" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="17" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -31,31 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
-  <si>
-    <t>Giám đốc công ty</t>
-  </si>
-  <si>
-    <t>Phó Giám Đốc</t>
-  </si>
-  <si>
-    <t>Phòng Tổng hợp</t>
-  </si>
-  <si>
-    <t>Trưởng phòng</t>
-  </si>
-  <si>
-    <t>Phó phòng</t>
-  </si>
-  <si>
-    <t>Chuyên viên Tổng hợp</t>
-  </si>
-  <si>
-    <t>Phòng Kinh doanh</t>
-  </si>
-  <si>
-    <t>Phòng Kỹ thuật</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>STT</t>
   </si>
@@ -75,64 +50,58 @@
     <t>Mô tả</t>
   </si>
   <si>
-    <t>Công ty ABC</t>
-  </si>
-  <si>
-    <t>Chuyên viên Kinh doanh</t>
-  </si>
-  <si>
-    <t>Chuyên viên Kỹ thuật</t>
-  </si>
-  <si>
-    <t>Tên công ty/phòng ban</t>
-  </si>
-  <si>
     <t>Tên chức danh</t>
   </si>
   <si>
-    <t>Mô tả Giám đốc</t>
-  </si>
-  <si>
-    <t>Mô tả trưởng phòng Tổng hợp</t>
-  </si>
-  <si>
-    <t>Mô tả Phó Giám đốc</t>
-  </si>
-  <si>
-    <t>GĐ</t>
-  </si>
-  <si>
-    <t>PGĐ</t>
-  </si>
-  <si>
-    <t>TP</t>
-  </si>
-  <si>
-    <t>PP</t>
-  </si>
-  <si>
-    <t>CV</t>
-  </si>
-  <si>
-    <t>Danh sách các đơn vị của : Công ty ABC</t>
-  </si>
-  <si>
-    <t>Tên</t>
-  </si>
-  <si>
-    <t>Chức danh chính</t>
-  </si>
-  <si>
-    <t>Chức danh kiêm nhiệm</t>
-  </si>
-  <si>
-    <t>Họ và chữ lót</t>
-  </si>
-  <si>
-    <t>Mã tổ chức</t>
+    <t>(Tên doanh nghiệp sẽ xuất ra ở đây)</t>
+  </si>
+  <si>
+    <t>DANH MỤC CƠ CẤU TỔ CHỨC CỦA:</t>
+  </si>
+  <si>
+    <t>DANH MỤC CƠ CẤU CHỨC DANH CỦA:</t>
+  </si>
+  <si>
+    <t>(Tên của doanh nghiệp ghi ở đây)</t>
   </si>
   <si>
     <t>Mã đơn vị</t>
+  </si>
+  <si>
+    <t>Tên Đơn vị</t>
+  </si>
+  <si>
+    <t>DANH SÁCH NHÂN VIÊN CỦA</t>
+  </si>
+  <si>
+    <t>(Tên tổ chức doang nghiệp ghi ở đây)</t>
+  </si>
+  <si>
+    <t>Họ và Tên</t>
+  </si>
+  <si>
+    <t>Mã Đơn vị</t>
+  </si>
+  <si>
+    <t>Tên viết tắt của Chức danh</t>
+  </si>
+  <si>
+    <t>Mô tả chức danh</t>
+  </si>
+  <si>
+    <t>Mã quản lý cấp trên</t>
+  </si>
+  <si>
+    <t>Mã chức danh chính</t>
+  </si>
+  <si>
+    <t>Tên chức danh chính</t>
+  </si>
+  <si>
+    <t>Mã các chức danh kiêm nhiệm</t>
+  </si>
+  <si>
+    <t>Tên các chức danh kiêm nhiệm</t>
   </si>
 </sst>
 </file>
@@ -142,7 +111,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -212,13 +181,30 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color rgb="FFFF0000"/>
+      <color theme="3" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="3" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -233,49 +219,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF66"/>
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -303,7 +259,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="1" diagonalDown="1">
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -313,16 +269,16 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom/>
-      <diagonal/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal style="thin">
+        <color auto="1"/>
+      </diagonal>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
+      <left/>
+      <right/>
       <top/>
       <bottom style="thin">
         <color auto="1"/>
@@ -330,14 +286,14 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
+      <left/>
       <right style="thin">
         <color auto="1"/>
       </right>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="1" diagonalDown="1">
@@ -347,12 +303,8 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal style="thin">
         <color auto="1"/>
       </diagonal>
@@ -393,43 +345,58 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="33">
     <cellStyle name="20% - Accent2 2" xfId="32" xr:uid="{9CCA8FE9-6B14-409D-8217-A36B47B0E62F}"/>
@@ -807,18 +774,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{838C49C0-4525-4B19-A798-BE216164A953}">
-  <dimension ref="A3:I3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.875" customWidth="1"/>
-    <col min="2" max="4" width="17.5" customWidth="1"/>
-    <col min="5" max="5" width="17.75" style="4" customWidth="1"/>
-    <col min="6" max="6" width="11.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.875" customWidth="1"/>
+    <col min="3" max="3" width="12.875" customWidth="1"/>
+    <col min="4" max="4" width="29.75" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.25" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="16" style="1" customWidth="1"/>
     <col min="10" max="10" width="9.625" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="10.125" bestFit="1" customWidth="1"/>
@@ -832,29 +804,50 @@
     <col min="20" max="20" width="5.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+    <row r="1" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>11</v>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+    </row>
+    <row r="2" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="H3"/>
       <c r="I3"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -862,70 +855,74 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050F21C7-B13B-48FF-8FB8-BF51E193B86B}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.25" customWidth="1"/>
+    <col min="3" max="3" width="12.375" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="9.25" customWidth="1"/>
+    <col min="6" max="6" width="11.625" customWidth="1"/>
+    <col min="7" max="7" width="11.25" customWidth="1"/>
+    <col min="8" max="8" width="10.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="6"/>
+    <row r="1" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="6"/>
+    <row r="2" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="16"/>
-      <c r="E3" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="6"/>
-    </row>
-    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="12" t="s">
+    <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="E3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>12</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B3:C3"/>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -933,265 +930,83 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C0E3A7-F6CF-41D7-A942-2E93BE0004DE}">
-  <dimension ref="A3:G3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.75" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.75" customWidth="1"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="8.125" customWidth="1"/>
+    <col min="4" max="4" width="16.5" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="7.5" customWidth="1"/>
+    <col min="7" max="7" width="9.375" customWidth="1"/>
+    <col min="8" max="8" width="7.875" customWidth="1"/>
+    <col min="9" max="9" width="10.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>32</v>
+    <row r="1" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+    </row>
+    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="9"/>
+    </row>
+    <row r="3" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD02D2ED-6AA4-4853-B69E-C166F4B46A85}">
-  <dimension ref="A3:G16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.25" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="16"/>
-      <c r="E3" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="19"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-      <c r="B7" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="19"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="19"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="19"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-      <c r="B10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="19"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="19"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="19"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="19"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="19"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="19"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="19"/>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A11:A13"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
edit all lan 3
</commit_message>
<xml_diff>
--- a/templates/sample-danhmuc-tochuc.xlsx
+++ b/templates/sample-danhmuc-tochuc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DINHNV\MyData\LAPTRINH\NODE4\ionic4.qlns\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94667082-D85F-4E39-B440-DC6BEA63EFD9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F811BDE1-8225-4593-A852-62452F470744}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3990" yWindow="555" windowWidth="17625" windowHeight="12405" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="organizations" sheetId="16" r:id="rId1"/>
@@ -776,7 +776,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{838C49C0-4525-4B19-A798-BE216164A953}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -861,19 +861,19 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.25" customWidth="1"/>
-    <col min="3" max="3" width="12.375" customWidth="1"/>
-    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="2" max="2" width="26.25" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="30.625" customWidth="1"/>
     <col min="5" max="5" width="9.25" customWidth="1"/>
     <col min="6" max="6" width="11.625" customWidth="1"/>
     <col min="7" max="7" width="11.25" customWidth="1"/>
-    <col min="8" max="8" width="10.25" customWidth="1"/>
+    <col min="8" max="8" width="32.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -893,7 +893,7 @@
       <c r="D2" s="15"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
@@ -932,24 +932,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C0E3A7-F6CF-41D7-A942-2E93BE0004DE}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.75" customWidth="1"/>
-    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="8.125" customWidth="1"/>
-    <col min="4" max="4" width="16.5" customWidth="1"/>
+    <col min="4" max="4" width="28.125" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="7.5" customWidth="1"/>
+    <col min="6" max="6" width="14.125" customWidth="1"/>
     <col min="7" max="7" width="9.375" customWidth="1"/>
-    <col min="8" max="8" width="7.875" customWidth="1"/>
-    <col min="9" max="9" width="10.125" customWidth="1"/>
+    <col min="8" max="8" width="20" customWidth="1"/>
+    <col min="9" max="9" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>